<commit_message>
Matrix multiplication with are more efficient now.
</commit_message>
<xml_diff>
--- a/lab3/time_counting.xlsx
+++ b/lab3/time_counting.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Cores</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Efficency</t>
   </si>
   <si>
+    <t>Base Size</t>
+  </si>
+  <si>
     <t>Size</t>
   </si>
   <si>
@@ -32,6 +35,9 @@
   </si>
   <si>
     <t>Slowdown</t>
+  </si>
+  <si>
+    <t>Base Processees</t>
   </si>
 </sst>
 </file>
@@ -102,7 +108,7 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -112,7 +118,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,7 +152,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>TIme относительно параметра "Cores"</a:t>
+              <a:t>Acceleration относительно параметра "Cores"</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -162,7 +168,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Лист1'!$B$1</c:f>
+              <c:f>'Лист1'!$C$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -177,22 +183,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Лист1'!$A$2:$A$11</c:f>
+              <c:f>'Лист1'!$A$2:$A$12</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Лист1'!$B$2:$B$11</c:f>
+              <c:f>'Лист1'!$C$2:$C$11</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2013085039"/>
-        <c:axId val="1792448551"/>
+        <c:axId val="1839158464"/>
+        <c:axId val="1316592355"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2013085039"/>
+        <c:axId val="1839158464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -244,10 +250,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1792448551"/>
+        <c:crossAx val="1316592355"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1792448551"/>
+        <c:axId val="1316592355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -294,7 +300,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>TIme</a:t>
+                  <a:t>Acceleration</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -322,7 +328,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2013085039"/>
+        <c:crossAx val="1839158464"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -372,7 +378,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Acceleration относительно параметра "Cores"</a:t>
+              <a:t>Efficency относительно параметра "Cores"</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -388,7 +394,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Лист1'!$C$1</c:f>
+              <c:f>'Лист1'!$D$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -403,22 +409,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Лист1'!$A$2:$A$11</c:f>
+              <c:f>'Лист1'!$A$2:$A$12</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Лист1'!$C$2:$C$11</c:f>
+              <c:f>'Лист1'!$D$2:$D$11</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="717152724"/>
-        <c:axId val="2081149201"/>
+        <c:axId val="1635075735"/>
+        <c:axId val="95049824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="717152724"/>
+        <c:axId val="1635075735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,10 +476,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081149201"/>
+        <c:crossAx val="95049824"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081149201"/>
+        <c:axId val="95049824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +526,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Acceleration</a:t>
+                  <a:t>Efficency</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -548,7 +554,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="717152724"/>
+        <c:crossAx val="1635075735"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -598,232 +604,6 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Efficency относительно параметра "Cores"</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Лист1'!$D$1</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="4285F4"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Лист1'!$A$2:$A$11</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Лист1'!$D$2:$D$11</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="663332193"/>
-        <c:axId val="811416120"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="663332193"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Cores</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="811416120"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="811416120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Efficency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="663332193"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
               <a:t>Slowdown относительно параметра "Size"</a:t>
             </a:r>
           </a:p>
@@ -866,11 +646,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1388954700"/>
-        <c:axId val="233946648"/>
+        <c:axId val="1327426644"/>
+        <c:axId val="771759535"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1388954700"/>
+        <c:axId val="1327426644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,10 +702,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233946648"/>
+        <c:crossAx val="771759535"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233946648"/>
+        <c:axId val="771759535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,7 +780,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1388954700"/>
+        <c:crossAx val="1327426644"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1026,7 +806,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1091,11 +871,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="183991358"/>
-        <c:axId val="1334389442"/>
+        <c:axId val="1297612550"/>
+        <c:axId val="2105304177"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183991358"/>
+        <c:axId val="1297612550"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,10 +927,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1334389442"/>
+        <c:crossAx val="2105304177"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1334389442"/>
+        <c:axId val="2105304177"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,7 +1005,233 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183991358"/>
+        <c:crossAx val="1297612550"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>TIme относительно параметра "Cores"</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Лист1'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Лист1'!$A$2:$A$12</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Лист1'!$B$2:$B$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="524546728"/>
+        <c:axId val="1784377813"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="524546728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Cores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1784377813"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1784377813"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>TIme</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524546728"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1255,12 +1261,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5076825" cy="3133725"/>
+    <xdr:ext cx="5010150" cy="3133725"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1" name="Chart 1" title="Диаграмма"/>
@@ -1280,12 +1286,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5010150" cy="3133725"/>
+    <xdr:ext cx="4914900" cy="3038475"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2" title="Диаграмма"/>
@@ -1305,12 +1311,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4914900" cy="3038475"/>
+    <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 3" title="Диаграмма"/>
@@ -1330,8 +1336,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
@@ -1355,12 +1361,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:ext cx="5095875" cy="3133725"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 5" title="Диаграмма"/>
@@ -1598,14 +1604,20 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -1613,7 +1625,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5">
-        <v>85.420566</v>
+        <v>69.306115</v>
       </c>
       <c r="C2" s="6">
         <f t="shared" ref="C2:C11" si="1">B$2/B2</f>
@@ -1623,15 +1635,21 @@
         <f t="shared" ref="D2:D11" si="2">C2/A2</f>
         <v>1</v>
       </c>
+      <c r="E2" s="3">
+        <v>1920.0</v>
+      </c>
       <c r="F2" s="3">
         <v>1600.0</v>
       </c>
       <c r="G2" s="3">
-        <v>9.69808</v>
+        <v>5.279359</v>
       </c>
       <c r="H2" s="6">
         <f t="shared" ref="H2:H6" si="3">G$2/G2</f>
         <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
@@ -1639,25 +1657,25 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="5">
-        <v>50.882678</v>
+        <v>35.222477</v>
       </c>
       <c r="C3" s="6">
         <f t="shared" si="1"/>
-        <v>1.678774965</v>
+        <v>1.967667265</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" si="2"/>
-        <v>0.8393874827</v>
+        <v>0.9838336327</v>
       </c>
       <c r="F3" s="3">
         <v>1760.0</v>
       </c>
       <c r="G3" s="3">
-        <v>10.821591</v>
+        <v>7.195129</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" si="3"/>
-        <v>0.8961787597</v>
+        <v>0.7337407015</v>
       </c>
     </row>
     <row r="4">
@@ -1665,25 +1683,25 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5">
-        <v>29.439435</v>
+        <v>23.535945</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" si="1"/>
-        <v>2.901569476</v>
+        <v>2.944692257</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="2"/>
-        <v>0.9671898255</v>
+        <v>0.9815640856</v>
       </c>
       <c r="F4" s="3">
         <v>1920.0</v>
       </c>
       <c r="G4" s="3">
-        <v>17.043771</v>
+        <v>9.107202</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" si="3"/>
-        <v>0.5690102267</v>
+        <v>0.579690557</v>
       </c>
     </row>
     <row r="5">
@@ -1691,25 +1709,25 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="5">
-        <v>25.446253</v>
+        <v>17.577833</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="1"/>
-        <v>3.356901545</v>
+        <v>3.942813372</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="2"/>
-        <v>0.8392253862</v>
+        <v>0.985703343</v>
       </c>
       <c r="F5" s="3">
         <v>2400.0</v>
       </c>
       <c r="G5" s="7">
-        <v>29.959929</v>
+        <v>17.752965</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="3"/>
-        <v>0.3237017017</v>
+        <v>0.2973790012</v>
       </c>
     </row>
     <row r="6">
@@ -1717,25 +1735,25 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="5">
-        <v>18.790283</v>
+        <v>14.51565</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="1"/>
-        <v>4.545996779</v>
+        <v>4.774578817</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="2"/>
-        <v>0.9091993559</v>
+        <v>0.9549157633</v>
       </c>
       <c r="F6" s="3">
         <v>3200.0</v>
       </c>
       <c r="G6" s="3">
-        <v>78.787412</v>
+        <v>42.184793</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="3"/>
-        <v>0.1230917447</v>
+        <v>0.1251483917</v>
       </c>
     </row>
     <row r="7">
@@ -1743,15 +1761,15 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="5">
-        <v>15.506055</v>
+        <v>12.111825</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="1"/>
-        <v>5.508852252</v>
+        <v>5.722185963</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="2"/>
-        <v>0.9181420419</v>
+        <v>0.9536976605</v>
       </c>
     </row>
     <row r="8">
@@ -1759,15 +1777,15 @@
         <v>8.0</v>
       </c>
       <c r="B8" s="5">
-        <v>14.474874</v>
+        <v>9.107202</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="1"/>
-        <v>5.901299452</v>
+        <v>7.610033795</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="2"/>
-        <v>0.7376624315</v>
+        <v>0.9512542244</v>
       </c>
     </row>
     <row r="9">
@@ -1775,15 +1793,15 @@
         <v>10.0</v>
       </c>
       <c r="B9" s="5">
-        <v>9.513201</v>
+        <v>7.33803</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="1"/>
-        <v>8.979161273</v>
+        <v>9.444784908</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="2"/>
-        <v>0.8979161273</v>
+        <v>0.9444784908</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1791,16 +1809,16 @@
       <c r="A10" s="4">
         <v>12.0</v>
       </c>
-      <c r="B10" s="4">
-        <v>9.588264</v>
+      <c r="B10" s="5">
+        <v>6.272013</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="1"/>
-        <v>8.908866715</v>
+        <v>11.05005921</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="2"/>
-        <v>0.7424055595</v>
+        <v>0.9208382673</v>
       </c>
     </row>
     <row r="11">
@@ -1808,28 +1826,28 @@
         <v>16.0</v>
       </c>
       <c r="B11" s="5">
-        <v>7.235588</v>
+        <v>4.591297</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="1"/>
-        <v>11.80561497</v>
+        <v>15.09510602</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="2"/>
-        <v>0.7378509355</v>
+        <v>0.9434441265</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="5"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21">
       <c r="A21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="9"/>
+      <c r="A22" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>